<commit_message>
Aggiornamento per caricamento test case 445
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#200000SWHCGMXX/COMPUGROUP_MEDICAL_ITALIA_S.p.a/FPF/5.70/report-checklist.xlsx
+++ b/GATEWAY/A1#200000SWHCGMXX/COMPUGROUP_MEDICAL_ITALIA_S.p.a/FPF/5.70/report-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgm01-my.sharepoint.com/personal/daniele_romanazzi_cgm_com/Documents/Documenti/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgm01-my.sharepoint.com/personal/domenico_depinto_cgm_com/Documents/Desktop/validazione/da caricare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F07F68B6-C5A3-4597-8A7B-5DFE7846B1F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{1F24850C-8DFB-4B05-9D3A-C0BE7F771772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{812AD218-F0B5-4145-B260-3373C5B9D133}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1297" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1303" uniqueCount="482">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1845,6 +1845,15 @@
   </si>
   <si>
     <t>Non è possibile valorizzare il codice in questione con un valore diverso da S quindi l'utente non può mai incorrere in questo errore / scenario</t>
+  </si>
+  <si>
+    <t>2025-02-20T05:11:45Z</t>
+  </si>
+  <si>
+    <t>50ec7ce1e84f761c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190201.4.4.c9e46412a5b4a1da85f5c1d1851717bc580c50202e314f7832592e3d7865819c.299c4b7737^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -2627,6 +2636,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4002,10 +4015,10 @@
   <dimension ref="A1:W775"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B167" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B171" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A185" sqref="A185"/>
+      <selection pane="bottomRight" activeCell="J185" sqref="J185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5073,9 +5086,15 @@
       <c r="O29" s="29" t="s">
         <v>460</v>
       </c>
-      <c r="P29" s="29"/>
-      <c r="Q29" s="29"/>
-      <c r="R29" s="29"/>
+      <c r="P29" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="Q29" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="R29" s="29" t="s">
+        <v>66</v>
+      </c>
       <c r="S29" s="29" t="s">
         <v>461</v>
       </c>
@@ -11225,12 +11244,20 @@
       <c r="E185" s="32" t="s">
         <v>283</v>
       </c>
-      <c r="F185" s="33"/>
-      <c r="G185" s="33"/>
-      <c r="H185" s="33"/>
-      <c r="I185" s="40"/>
+      <c r="F185" s="33">
+        <v>45708</v>
+      </c>
+      <c r="G185" s="33" t="s">
+        <v>479</v>
+      </c>
+      <c r="H185" s="33" t="s">
+        <v>480</v>
+      </c>
+      <c r="I185" s="40" t="s">
+        <v>481</v>
+      </c>
       <c r="J185" s="29" t="s">
-        <v>267</v>
+        <v>66</v>
       </c>
       <c r="K185" s="29"/>
       <c r="L185" s="29"/>
@@ -11245,7 +11272,7 @@
       <c r="U185" s="34"/>
       <c r="V185" s="35"/>
       <c r="W185" s="29" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="186" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -18439,6 +18466,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca719f03-9e45-4ef4-9920-d156f53157f2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100F560B38A5B3C4B41B1895754B1F1A56A" ma:contentTypeVersion="9" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="69dc0f489d46816a4b9bb4a327e14425">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ca719f03-9e45-4ef4-9920-d156f53157f2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7de9a44ff87fdcabda187bbd662e75de" ns2:_="">
     <xsd:import namespace="ca719f03-9e45-4ef4-9920-d156f53157f2"/>
@@ -18610,26 +18656,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="ca719f03-9e45-4ef4-9920-d156f53157f2"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca719f03-9e45-4ef4-9920-d156f53157f2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61CEF28A-E0A2-4D9D-9130-F7D0F35034F1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18647,33 +18700,9 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ca719f03-9e45-4ef4-9920-d156f53157f2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>
-  <clbl:label id="{fbf47bbe-a0a2-4c04-9ba4-22f94012202d}" enabled="1" method="Standard" siteId="{69602cf4-a76e-4265-955f-03c329c50608}" removed="0"/>
+  <clbl:label id="{fbf47bbe-a0a2-4c04-9ba4-22f94012202d}" enabled="1" method="Standard" siteId="{69602cf4-a76e-4265-955f-03c329c50608}" contentBits="2" removed="0"/>
 </clbl:labelList>
 </file>
</xml_diff>